<commit_message>
14.12.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/December/Others/Draft Sales target -Rajshahi-December,2020 - Regional Feedback.xlsx
+++ b/2020/December/Others/Draft Sales target -Rajshahi-December,2020 - Regional Feedback.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Distributor Primary" sheetId="1" r:id="rId1"/>
@@ -1360,6 +1360,20 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="8" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1381,20 +1395,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="8" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="8" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1975,7 +1975,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1988,11 +1988,11 @@
   </sheetPr>
   <dimension ref="A1:AJ21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="AE7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AH14" sqref="AH14"/>
+      <selection pane="bottomRight" activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -3366,115 +3366,115 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="120" customFormat="1">
-      <c r="A14" s="115" t="s">
+    <row r="14" spans="1:36" s="113" customFormat="1">
+      <c r="A14" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="116" t="s">
+      <c r="B14" s="109" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="117">
+      <c r="C14" s="110">
         <f t="shared" si="0"/>
         <v>14038990.979181854</v>
       </c>
-      <c r="D14" s="117">
+      <c r="D14" s="110">
         <f t="shared" si="1"/>
         <v>9487</v>
       </c>
-      <c r="E14" s="118">
+      <c r="E14" s="111">
         <v>611</v>
       </c>
-      <c r="F14" s="118">
+      <c r="F14" s="111">
         <v>855</v>
       </c>
-      <c r="G14" s="118">
+      <c r="G14" s="111">
         <v>794</v>
       </c>
-      <c r="H14" s="118">
+      <c r="H14" s="111">
         <v>122</v>
       </c>
-      <c r="I14" s="118">
+      <c r="I14" s="111">
         <v>366</v>
       </c>
-      <c r="J14" s="118">
+      <c r="J14" s="111">
         <v>366</v>
       </c>
-      <c r="K14" s="118">
+      <c r="K14" s="111">
         <v>366</v>
       </c>
-      <c r="L14" s="118">
+      <c r="L14" s="111">
         <v>366</v>
       </c>
-      <c r="M14" s="118">
+      <c r="M14" s="111">
         <v>488</v>
       </c>
-      <c r="N14" s="118">
+      <c r="N14" s="111">
         <v>189</v>
       </c>
-      <c r="O14" s="118">
+      <c r="O14" s="111">
         <v>574</v>
       </c>
-      <c r="P14" s="118">
+      <c r="P14" s="111">
         <v>366</v>
       </c>
-      <c r="Q14" s="118">
+      <c r="Q14" s="111">
         <v>614</v>
       </c>
-      <c r="R14" s="118">
+      <c r="R14" s="111">
         <v>328</v>
       </c>
-      <c r="S14" s="118">
+      <c r="S14" s="111">
         <v>417</v>
       </c>
-      <c r="T14" s="118">
+      <c r="T14" s="111">
         <v>368</v>
       </c>
-      <c r="U14" s="118">
+      <c r="U14" s="111">
         <v>396</v>
       </c>
-      <c r="V14" s="118">
+      <c r="V14" s="111">
         <v>246</v>
       </c>
-      <c r="W14" s="118">
+      <c r="W14" s="111">
         <v>351</v>
       </c>
-      <c r="X14" s="118">
+      <c r="X14" s="111">
         <v>261</v>
       </c>
-      <c r="Y14" s="118">
+      <c r="Y14" s="111">
         <v>117</v>
       </c>
-      <c r="Z14" s="118">
+      <c r="Z14" s="111">
         <v>88</v>
       </c>
-      <c r="AA14" s="118">
+      <c r="AA14" s="111">
         <v>7</v>
       </c>
-      <c r="AB14" s="118">
+      <c r="AB14" s="111">
         <v>88</v>
       </c>
-      <c r="AC14" s="118">
+      <c r="AC14" s="111">
         <v>65</v>
       </c>
-      <c r="AD14" s="118">
+      <c r="AD14" s="111">
         <v>88</v>
       </c>
-      <c r="AE14" s="118">
+      <c r="AE14" s="111">
         <v>85</v>
       </c>
-      <c r="AF14" s="118">
+      <c r="AF14" s="111">
         <v>77</v>
       </c>
-      <c r="AG14" s="119">
+      <c r="AG14" s="112">
         <v>124</v>
       </c>
-      <c r="AH14" s="118">
+      <c r="AH14" s="111">
         <v>209</v>
       </c>
-      <c r="AI14" s="115">
+      <c r="AI14" s="108">
         <v>88</v>
       </c>
-      <c r="AJ14" s="115">
+      <c r="AJ14" s="108">
         <v>7</v>
       </c>
     </row>
@@ -4151,10 +4151,10 @@
       </c>
     </row>
     <row r="21" spans="1:36">
-      <c r="A21" s="108" t="s">
+      <c r="A21" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="108"/>
+      <c r="B21" s="114"/>
       <c r="C21" s="14">
         <f>SUM(C4:C20)</f>
         <v>152678127.55783212</v>
@@ -6479,10 +6479,10 @@
       </c>
     </row>
     <row r="21" spans="1:36">
-      <c r="A21" s="108" t="s">
+      <c r="A21" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="108"/>
+      <c r="B21" s="114"/>
       <c r="C21" s="14">
         <f t="shared" ref="C21:AJ21" si="2">SUM(C4:C20)</f>
         <v>156216155</v>
@@ -6638,11 +6638,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -7763,10 +7763,10 @@
       </c>
     </row>
     <row r="10" spans="1:36">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="108"/>
+      <c r="B10" s="114"/>
       <c r="C10" s="14">
         <f>SUM(C4:C9)</f>
         <v>156216155</v>
@@ -7960,25 +7960,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:91" ht="12.75">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="109" t="s">
+      <c r="F1" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="109" t="s">
+      <c r="G1" s="115" t="s">
         <v>43</v>
       </c>
       <c r="H1" s="6">
@@ -8079,13 +8079,13 @@
       </c>
     </row>
     <row r="2" spans="1:91" ht="12.75">
-      <c r="A2" s="111"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
+      <c r="A2" s="117"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
@@ -22388,25 +22388,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="118" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="118" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="109" t="s">
+      <c r="F1" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="109" t="s">
+      <c r="G1" s="115" t="s">
         <v>43</v>
       </c>
       <c r="H1" s="81">
@@ -22507,13 +22507,13 @@
       </c>
     </row>
     <row r="2" spans="1:39">
-      <c r="A2" s="111"/>
-      <c r="B2" s="113"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
+      <c r="A2" s="117"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
       <c r="H2" s="83" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
22.12.2020 MC SAles Details
</commit_message>
<xml_diff>
--- a/2020/December/Others/Draft Sales target -Rajshahi-December,2020 - Regional Feedback.xlsx
+++ b/2020/December/Others/Draft Sales target -Rajshahi-December,2020 - Regional Feedback.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Distributor Primary" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="254">
   <si>
     <t>DP</t>
   </si>
@@ -789,6 +789,9 @@
   <si>
     <t>Md. Babu</t>
   </si>
+  <si>
+    <t>21.12.2020</t>
+  </si>
 </sst>
 </file>
 
@@ -906,7 +909,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -970,6 +973,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1110,7 +1119,7 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1395,6 +1404,10 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1975,7 +1988,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1986,13 +1999,13 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:AJ21"/>
+  <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="AE7" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="I14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AI14" sqref="AI14"/>
+      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2026,7 +2039,8 @@
     <col min="33" max="33" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="19.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="4"/>
+    <col min="37" max="37" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="14.25">
@@ -2246,7 +2260,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" hidden="1">
       <c r="A4" s="13" t="s">
         <v>19</v>
       </c>
@@ -2358,7 +2372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" hidden="1">
       <c r="A5" s="13" t="s">
         <v>21</v>
       </c>
@@ -2470,7 +2484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" hidden="1">
       <c r="A6" s="13" t="s">
         <v>22</v>
       </c>
@@ -2582,7 +2596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" hidden="1">
       <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
@@ -2694,7 +2708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" hidden="1">
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
@@ -2806,7 +2820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" hidden="1">
       <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
@@ -2918,7 +2932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" hidden="1">
       <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
@@ -3030,7 +3044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" hidden="1">
       <c r="A11" s="13" t="s">
         <v>27</v>
       </c>
@@ -3142,7 +3156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" hidden="1">
       <c r="A12" s="13" t="s">
         <v>28</v>
       </c>
@@ -3254,7 +3268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" hidden="1">
       <c r="A13" s="13" t="s">
         <v>29</v>
       </c>
@@ -3478,7 +3492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" hidden="1">
       <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
@@ -3590,7 +3604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" hidden="1">
       <c r="A16" s="13" t="s">
         <v>32</v>
       </c>
@@ -3702,7 +3716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:37" hidden="1">
       <c r="A17" s="13" t="s">
         <v>33</v>
       </c>
@@ -3814,7 +3828,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:37" hidden="1">
       <c r="A18" s="13" t="s">
         <v>34</v>
       </c>
@@ -3926,7 +3940,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:37" hidden="1">
       <c r="A19" s="13" t="s">
         <v>35</v>
       </c>
@@ -4038,7 +4052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:37" hidden="1">
       <c r="A20" s="13" t="s">
         <v>36</v>
       </c>
@@ -4150,7 +4164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:37" hidden="1">
       <c r="A21" s="114" t="s">
         <v>37</v>
       </c>
@@ -4290,6 +4304,444 @@
       <c r="AJ21" s="14">
         <f t="shared" si="2"/>
         <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>450</v>
+      </c>
+      <c r="G22" s="3">
+        <v>680</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>300</v>
+      </c>
+      <c r="J22" s="3">
+        <v>400</v>
+      </c>
+      <c r="K22" s="3">
+        <v>300</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="M22" s="3">
+        <v>40</v>
+      </c>
+      <c r="N22" s="3">
+        <v>180</v>
+      </c>
+      <c r="O22" s="3">
+        <v>200</v>
+      </c>
+      <c r="P22" s="3">
+        <v>404</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>260</v>
+      </c>
+      <c r="R22" s="3">
+        <v>357</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0</v>
+      </c>
+      <c r="T22" s="3">
+        <v>0</v>
+      </c>
+      <c r="U22" s="3">
+        <v>363</v>
+      </c>
+      <c r="V22" s="3">
+        <v>260</v>
+      </c>
+      <c r="W22" s="3">
+        <v>100</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>50</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="3">
+        <v>40</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>20</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>40</v>
+      </c>
+      <c r="AE22" s="3">
+        <v>65</v>
+      </c>
+      <c r="AF22" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG22" s="3">
+        <v>200</v>
+      </c>
+      <c r="AH22" s="3">
+        <v>140</v>
+      </c>
+      <c r="AI22" s="4">
+        <v>40</v>
+      </c>
+      <c r="AJ22" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="E23" s="121">
+        <f>E14-E22</f>
+        <v>611</v>
+      </c>
+      <c r="F23" s="121">
+        <f t="shared" ref="F23:AJ23" si="3">F14-F22</f>
+        <v>405</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="3"/>
+        <v>114</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="3"/>
+        <v>122</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="3"/>
+        <v>-34</v>
+      </c>
+      <c r="K23" s="121">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="3"/>
+        <v>366</v>
+      </c>
+      <c r="M23" s="121">
+        <f t="shared" si="3"/>
+        <v>448</v>
+      </c>
+      <c r="N23" s="121">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="O23" s="121">
+        <f t="shared" si="3"/>
+        <v>374</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" si="3"/>
+        <v>-38</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="3"/>
+        <v>354</v>
+      </c>
+      <c r="R23" s="3">
+        <f t="shared" si="3"/>
+        <v>-29</v>
+      </c>
+      <c r="S23" s="121">
+        <f t="shared" si="3"/>
+        <v>417</v>
+      </c>
+      <c r="T23" s="3">
+        <f t="shared" si="3"/>
+        <v>368</v>
+      </c>
+      <c r="U23" s="3">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="V23" s="3">
+        <f t="shared" si="3"/>
+        <v>-14</v>
+      </c>
+      <c r="W23" s="3">
+        <f t="shared" si="3"/>
+        <v>251</v>
+      </c>
+      <c r="X23" s="121">
+        <f t="shared" si="3"/>
+        <v>261</v>
+      </c>
+      <c r="Y23" s="3">
+        <f t="shared" si="3"/>
+        <v>117</v>
+      </c>
+      <c r="Z23" s="3">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="AA23" s="121">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="AB23" s="3">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="AC23" s="3">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="AD23" s="121">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="AE23" s="3">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="AF23" s="3">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+      <c r="AG23" s="3">
+        <f t="shared" si="3"/>
+        <v>-76</v>
+      </c>
+      <c r="AH23" s="3">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="AI23" s="121">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="AJ23" s="3">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="E24" s="3">
+        <v>200</v>
+      </c>
+      <c r="F24" s="3">
+        <v>200</v>
+      </c>
+      <c r="G24" s="3">
+        <v>200</v>
+      </c>
+      <c r="H24" s="3">
+        <v>140</v>
+      </c>
+      <c r="I24" s="3">
+        <v>100</v>
+      </c>
+      <c r="L24" s="3">
+        <v>400</v>
+      </c>
+      <c r="M24" s="3">
+        <v>300</v>
+      </c>
+      <c r="N24" s="3">
+        <v>40</v>
+      </c>
+      <c r="O24" s="3">
+        <v>100</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>400</v>
+      </c>
+      <c r="T24" s="3">
+        <v>400</v>
+      </c>
+      <c r="U24" s="3">
+        <v>100</v>
+      </c>
+      <c r="W24" s="3">
+        <v>200</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>120</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>40</v>
+      </c>
+      <c r="AB24" s="3">
+        <v>40</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>40</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>40</v>
+      </c>
+      <c r="AE24" s="3">
+        <v>40</v>
+      </c>
+      <c r="AF24" s="3">
+        <v>100</v>
+      </c>
+      <c r="AG24" s="3">
+        <v>100</v>
+      </c>
+      <c r="AH24" s="3">
+        <v>80</v>
+      </c>
+      <c r="AI24" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="E25" s="3">
+        <f>E24*E2</f>
+        <v>152301.11642975363</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" ref="F25:AJ25" si="4">F24*F2</f>
+        <v>154325.64464533899</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="4"/>
+        <v>148574.83244755262</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="4"/>
+        <v>128387.29786072395</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="4"/>
+        <v>81520.227808219061</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="4"/>
+        <v>374987.3311553775</v>
+      </c>
+      <c r="M25" s="3">
+        <f t="shared" si="4"/>
+        <v>280813.7883802813</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" si="4"/>
+        <v>40677.248322147636</v>
+      </c>
+      <c r="O25" s="3">
+        <f t="shared" si="4"/>
+        <v>96601.04866336644</v>
+      </c>
+      <c r="P25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="3">
+        <f t="shared" si="4"/>
+        <v>468770.17431034299</v>
+      </c>
+      <c r="R25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="S25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="3">
+        <f t="shared" si="4"/>
+        <v>429207.61538461584</v>
+      </c>
+      <c r="U25" s="3">
+        <f t="shared" si="4"/>
+        <v>112184.70922123855</v>
+      </c>
+      <c r="V25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W25" s="3">
+        <f t="shared" si="4"/>
+        <v>246002.70186588942</v>
+      </c>
+      <c r="X25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y25" s="3">
+        <f t="shared" si="4"/>
+        <v>142964.51999999981</v>
+      </c>
+      <c r="Z25" s="3">
+        <f t="shared" si="4"/>
+        <v>142054.50711839655</v>
+      </c>
+      <c r="AA25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="3">
+        <f t="shared" si="4"/>
+        <v>158028.37804477772</v>
+      </c>
+      <c r="AC25" s="3">
+        <f t="shared" si="4"/>
+        <v>162072.80010921505</v>
+      </c>
+      <c r="AD25" s="3">
+        <f t="shared" si="4"/>
+        <v>202346.92974850256</v>
+      </c>
+      <c r="AE25" s="3">
+        <f t="shared" si="4"/>
+        <v>232232.04710810835</v>
+      </c>
+      <c r="AF25" s="3">
+        <f t="shared" si="4"/>
+        <v>642014.23792387859</v>
+      </c>
+      <c r="AG25" s="3">
+        <f t="shared" si="4"/>
+        <v>762358.76882352959</v>
+      </c>
+      <c r="AH25" s="3">
+        <f t="shared" si="4"/>
+        <v>660248.39944554213</v>
+      </c>
+      <c r="AI25" s="3">
+        <f t="shared" si="4"/>
+        <v>363171.29739486956</v>
+      </c>
+      <c r="AJ25" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AK25" s="122">
+        <f>SUM(E25:AJ25)</f>
+        <v>6181845.6222116677</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="J32" s="3" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -6638,11 +7090,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R25" sqref="R25"/>
+      <selection pane="bottomRight" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>

</xml_diff>